<commit_message>
work on import pointsourceactivities
</commit_message>
<xml_diff>
--- a/tests/edb/data/EMEPemissionfactors-short.xlsx
+++ b/tests/edb/data/EMEPemissionfactors-short.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="79">
   <si>
     <t xml:space="preserve">NFR</t>
   </si>
@@ -218,6 +218,45 @@
   </si>
   <si>
     <t xml:space="preserve">US EPA (1998), chapter 1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A.4.b.i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residential plants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advanced coal combustion techniques &lt;1MWth - Advanced stove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coal Fuels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kakareka et al. (2004)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.A.4.b.ii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Household and gardening (mobile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table_3-1_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier 1 emission factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">g/tonnes fuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Winther 2016</t>
   </si>
 </sst>
 </file>
@@ -232,6 +271,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -317,13 +357,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W11"/>
+  <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="12:13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -887,6 +927,104 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>260</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>6720</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>